<commit_message>
Q1 2023 Fiscal Data update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BTr-NG-COR-Latest.xlsx
+++ b/Data/Fiscal Data/BTr-NG-COR-Latest.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Joann\COR 2004-2022\COR 2022\corFY2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R-Projects\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B64B968-ED3A-42C9-9184-89791B29C5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118F46BF-5D45-40E6-B16C-4ECDE1C9A11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="13110" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2022 v2" sheetId="1" r:id="rId1"/>
+    <sheet name="2023" sheetId="2" r:id="rId1"/>
+    <sheet name="2022 v2" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'2022 v2'!$A$1:$R$61</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'2022 v2'!$A$1:$R$61</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'2023'!$A$1:$I$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
   <si>
     <t>National Government Cash Operation Report</t>
   </si>
@@ -291,6 +293,12 @@
   <si>
     <t>Dec</t>
   </si>
+  <si>
+    <t>CY 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amortization    </t>
+  </si>
 </sst>
 </file>
 
@@ -299,7 +307,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +413,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -449,12 +464,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -522,10 +538,36 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="37" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="37" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 11" xfId="3" xr:uid="{BF49F760-2DD8-4DB3-A84F-9281570256C0}"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -803,10 +845,910 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7AAED26-1E8C-4704-9ABA-F18595CCE15F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
+      <pane xSplit="5" ySplit="7" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="F39" sqref="F39:H39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="1.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="1.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:9" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="6.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8">
+        <f t="shared" ref="F9:I9" si="0">+F10+F21+F28</f>
+        <v>348167.25</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="0"/>
+        <v>211868</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="0"/>
+        <v>258650</v>
+      </c>
+      <c r="I9" s="8">
+        <f t="shared" si="0"/>
+        <v>818685.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" ref="F10:I10" si="1">+F11+F16+F19</f>
+        <v>305431</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="1"/>
+        <v>192290</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" si="1"/>
+        <v>221793</v>
+      </c>
+      <c r="I10" s="8">
+        <f t="shared" si="1"/>
+        <v>719514</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="9">
+        <v>234819</v>
+      </c>
+      <c r="G11" s="9">
+        <v>129378</v>
+      </c>
+      <c r="H11" s="9">
+        <v>140962</v>
+      </c>
+      <c r="I11" s="9">
+        <f>SUM(F11+G11+H11)</f>
+        <v>505159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="37">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>646</v>
+      </c>
+      <c r="H13" s="9">
+        <v>2704</v>
+      </c>
+      <c r="I13" s="9">
+        <f t="shared" ref="I13:I14" si="2">SUM(F13+G13+H13)</f>
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="9">
+        <v>723</v>
+      </c>
+      <c r="G14" s="9">
+        <v>5</v>
+      </c>
+      <c r="H14" s="9">
+        <v>40</v>
+      </c>
+      <c r="I14" s="9">
+        <f t="shared" si="2"/>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="38">
+        <v>70591</v>
+      </c>
+      <c r="G16" s="9">
+        <v>62895</v>
+      </c>
+      <c r="H16" s="9">
+        <v>80343</v>
+      </c>
+      <c r="I16" s="9">
+        <f>SUM(F16+G16+H16)</f>
+        <v>213829</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="37">
+        <v>0</v>
+      </c>
+      <c r="G18" s="9">
+        <v>132</v>
+      </c>
+      <c r="H18" s="9">
+        <v>46</v>
+      </c>
+      <c r="I18" s="9">
+        <f t="shared" ref="I18:I19" si="3">SUM(F18+G18+H18)</f>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="38">
+        <v>21</v>
+      </c>
+      <c r="G19" s="9">
+        <v>17</v>
+      </c>
+      <c r="H19" s="9">
+        <v>488</v>
+      </c>
+      <c r="I19" s="9">
+        <f t="shared" si="3"/>
+        <v>526</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="8">
+        <f t="shared" ref="F21:I21" si="4">SUM(F22:F26)</f>
+        <v>42726</v>
+      </c>
+      <c r="G21" s="8">
+        <f t="shared" si="4"/>
+        <v>19578</v>
+      </c>
+      <c r="H21" s="8">
+        <f t="shared" si="4"/>
+        <v>36857</v>
+      </c>
+      <c r="I21" s="8">
+        <f t="shared" si="4"/>
+        <v>99161</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="9">
+        <v>17753</v>
+      </c>
+      <c r="G22" s="9">
+        <v>6398</v>
+      </c>
+      <c r="H22" s="9">
+        <v>14873</v>
+      </c>
+      <c r="I22" s="9">
+        <f t="shared" ref="I22:I26" si="5">SUM(F22+G22+H22)</f>
+        <v>39024</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="39">
+        <f>939-939+1409+701</f>
+        <v>2110</v>
+      </c>
+      <c r="G23" s="39">
+        <f>574+654</f>
+        <v>1228</v>
+      </c>
+      <c r="H23" s="39">
+        <v>531</v>
+      </c>
+      <c r="I23" s="9">
+        <f t="shared" si="5"/>
+        <v>3869</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0</v>
+      </c>
+      <c r="G24" s="9">
+        <v>22</v>
+      </c>
+      <c r="H24" s="9">
+        <v>6</v>
+      </c>
+      <c r="I24" s="9">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="38">
+        <v>10514</v>
+      </c>
+      <c r="G25" s="9">
+        <v>2077</v>
+      </c>
+      <c r="H25" s="9">
+        <v>1653</v>
+      </c>
+      <c r="I25" s="9">
+        <f t="shared" si="5"/>
+        <v>14244</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="9">
+        <v>12349</v>
+      </c>
+      <c r="G26" s="9">
+        <v>9853</v>
+      </c>
+      <c r="H26" s="9">
+        <v>19794</v>
+      </c>
+      <c r="I26" s="9">
+        <f t="shared" si="5"/>
+        <v>41996</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="9">
+        <v>10.25</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0</v>
+      </c>
+      <c r="I28" s="9">
+        <f>SUM(F28+G28+H28)</f>
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8">
+        <f t="shared" ref="F30:I30" si="6">SUM(F31:F37)</f>
+        <v>302418</v>
+      </c>
+      <c r="G30" s="8">
+        <f t="shared" si="6"/>
+        <v>318241</v>
+      </c>
+      <c r="H30" s="8">
+        <f t="shared" si="6"/>
+        <v>468911</v>
+      </c>
+      <c r="I30" s="8">
+        <f t="shared" si="6"/>
+        <v>1089570</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="9">
+        <v>73752</v>
+      </c>
+      <c r="G31" s="9">
+        <v>73834</v>
+      </c>
+      <c r="H31" s="9">
+        <v>83271</v>
+      </c>
+      <c r="I31" s="9">
+        <f t="shared" ref="I31:I37" si="7">SUM(F31+G31+H31)</f>
+        <v>230857</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="9">
+        <v>46970</v>
+      </c>
+      <c r="G32" s="9">
+        <v>34109</v>
+      </c>
+      <c r="H32" s="9">
+        <v>60898</v>
+      </c>
+      <c r="I32" s="9">
+        <f t="shared" si="7"/>
+        <v>141977</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="9">
+        <f>F13+F14+F18</f>
+        <v>723</v>
+      </c>
+      <c r="G33" s="9">
+        <f>G13+G14+G18</f>
+        <v>783</v>
+      </c>
+      <c r="H33" s="9">
+        <f>H13+H14+H18</f>
+        <v>2790</v>
+      </c>
+      <c r="I33" s="9">
+        <f t="shared" si="7"/>
+        <v>4296</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="9">
+        <v>1112</v>
+      </c>
+      <c r="G34" s="9">
+        <v>9401</v>
+      </c>
+      <c r="H34" s="9">
+        <v>10795</v>
+      </c>
+      <c r="I34" s="9">
+        <f t="shared" si="7"/>
+        <v>21308</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="9">
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <v>11</v>
+      </c>
+      <c r="H35" s="9">
+        <v>106</v>
+      </c>
+      <c r="I35" s="9">
+        <f t="shared" si="7"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="9">
+        <v>0</v>
+      </c>
+      <c r="G36" s="9">
+        <v>12</v>
+      </c>
+      <c r="H36" s="9">
+        <v>628</v>
+      </c>
+      <c r="I36" s="9">
+        <f t="shared" si="7"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="D37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F37" s="9">
+        <f>157549+23035-F33</f>
+        <v>179861</v>
+      </c>
+      <c r="G37" s="9">
+        <f>175407+25467-G33</f>
+        <v>200091</v>
+      </c>
+      <c r="H37" s="9">
+        <f>280904+32309-H33</f>
+        <v>310423</v>
+      </c>
+      <c r="I37" s="9">
+        <f t="shared" si="7"/>
+        <v>690375</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="10">
+        <f>+F9-F30</f>
+        <v>45749.25</v>
+      </c>
+      <c r="G39" s="10">
+        <f>+G9-G30</f>
+        <v>-106373</v>
+      </c>
+      <c r="H39" s="10">
+        <f>+H9-H30</f>
+        <v>-210261</v>
+      </c>
+      <c r="I39" s="10">
+        <f>+I9-I30</f>
+        <v>-270884.75</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="B41" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="8">
+        <f t="shared" ref="F41:I41" si="8">+F42+F46</f>
+        <v>366005</v>
+      </c>
+      <c r="G41" s="8">
+        <f t="shared" si="8"/>
+        <v>305339</v>
+      </c>
+      <c r="H41" s="8">
+        <f t="shared" si="8"/>
+        <v>229432</v>
+      </c>
+      <c r="I41" s="8">
+        <f t="shared" si="8"/>
+        <v>900776</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" s="11">
+        <f t="shared" ref="F42:I42" si="9">+F43-F44</f>
+        <v>186705</v>
+      </c>
+      <c r="G42" s="11">
+        <f t="shared" si="9"/>
+        <v>-22160</v>
+      </c>
+      <c r="H42" s="11">
+        <f t="shared" si="9"/>
+        <v>83645</v>
+      </c>
+      <c r="I42" s="11">
+        <f t="shared" si="9"/>
+        <v>248190</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" s="9">
+        <v>187563</v>
+      </c>
+      <c r="G43" s="9">
+        <v>15984</v>
+      </c>
+      <c r="H43" s="9">
+        <v>91557</v>
+      </c>
+      <c r="I43" s="9">
+        <f>SUM(F43+G43+H43)</f>
+        <v>295104</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="9">
+        <v>858</v>
+      </c>
+      <c r="G44" s="9">
+        <v>38144</v>
+      </c>
+      <c r="H44" s="9">
+        <v>7912</v>
+      </c>
+      <c r="I44" s="9">
+        <f>SUM(F44+G44+H44)</f>
+        <v>46914</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="C46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" s="8">
+        <f t="shared" ref="F46:I46" si="10">+F47-F48</f>
+        <v>179300</v>
+      </c>
+      <c r="G46" s="8">
+        <f t="shared" si="10"/>
+        <v>327499</v>
+      </c>
+      <c r="H46" s="8">
+        <f t="shared" si="10"/>
+        <v>145787</v>
+      </c>
+      <c r="I46" s="8">
+        <f t="shared" si="10"/>
+        <v>652586</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D47" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F47" s="9">
+        <v>179300</v>
+      </c>
+      <c r="G47" s="9">
+        <v>359313</v>
+      </c>
+      <c r="H47" s="9">
+        <v>146045</v>
+      </c>
+      <c r="I47" s="9">
+        <f>SUM(F47+G47+H47)</f>
+        <v>684658</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F48" s="40">
+        <f t="shared" ref="F48:H48" si="11">F49-F50</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="40">
+        <f t="shared" si="11"/>
+        <v>31814</v>
+      </c>
+      <c r="H48" s="40">
+        <f t="shared" si="11"/>
+        <v>258</v>
+      </c>
+      <c r="I48" s="40">
+        <f>I49-I50</f>
+        <v>32072</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E49" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F49" s="9">
+        <v>3</v>
+      </c>
+      <c r="G49" s="9">
+        <v>303461</v>
+      </c>
+      <c r="H49" s="9">
+        <v>73361</v>
+      </c>
+      <c r="I49" s="9">
+        <f>SUM(F49+G49+H49)</f>
+        <v>376825</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="E50" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F50" s="9">
+        <v>3</v>
+      </c>
+      <c r="G50" s="9">
+        <v>271647</v>
+      </c>
+      <c r="H50" s="9">
+        <v>73103</v>
+      </c>
+      <c r="I50" s="9">
+        <f>SUM(F50+G50+H50)</f>
+        <v>344753</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+    </row>
+    <row r="52" spans="1:12" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" s="10">
+        <v>590732</v>
+      </c>
+      <c r="G52" s="10">
+        <v>-161942</v>
+      </c>
+      <c r="H52" s="10">
+        <v>492513</v>
+      </c>
+      <c r="I52" s="10">
+        <f>SUM(F52+G52+H52)</f>
+        <v>921303</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="9"/>
+    </row>
+    <row r="54" spans="1:12" s="15" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" s="14"/>
+    </row>
+    <row r="55" spans="1:12" s="15" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+    </row>
+    <row r="56" spans="1:12" s="15" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="42"/>
+      <c r="D56" s="42"/>
+      <c r="E56" s="42"/>
+      <c r="F56" s="42"/>
+    </row>
+    <row r="57" spans="1:12" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B57" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="45"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="46"/>
+    </row>
+    <row r="58" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="47"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="48"/>
+      <c r="F58" s="48"/>
+    </row>
+    <row r="59" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A60" s="20"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="L60" s="23"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" s="6"/>
+    </row>
+    <row r="62" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="24"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="vUKvUja6pFu/OeiT7bIoyFlIazUQbO3iZpEN9Y+L85D/s/y/nSJtNjq9gm06KH9dj2J9A3yCKHMcC7fQ2qGV5Q==" saltValue="DGGXUDuiN0lrqnYxoP5s0Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0" right="0" top="0.78740157480314965" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"-,Bold"&amp;10BUREAU OF THE TREASURY&amp;11
+&amp;"-,Italic"&amp;9 Statistical Data Analysis Division</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
       <pane xSplit="5" ySplit="7" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>

</xml_diff>